<commit_message>
akeaneo connector more test
</commit_message>
<xml_diff>
--- a/Akeneo Test Data.xlsx
+++ b/Akeneo Test Data.xlsx
@@ -5,24 +5,25 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cerdamario13\Documents\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cerdamario13\Documents\Python Files\WranglesPy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85D2A6C-6E29-4F94-97A3-CEF22B7923E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAC406C-2FFF-4A5A-A7EB-E16E9F26198D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27300" yWindow="615" windowWidth="24120" windowHeight="13170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28020" yWindow="375" windowWidth="27735" windowHeight="11895" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Read" sheetId="1" r:id="rId1"/>
     <sheet name="Data to Write Test 1" sheetId="3" r:id="rId2"/>
-    <sheet name="Data to Write ALL" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="11" r:id="rId3"/>
+    <sheet name="Data to Write ALL" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="61">
   <si>
     <t>identifier</t>
   </si>
@@ -153,12 +154,6 @@
     <t>Group_2</t>
   </si>
   <si>
-    <t>Currency</t>
-  </si>
-  <si>
-    <t>Amount</t>
-  </si>
-  <si>
     <t>Item1</t>
   </si>
   <si>
@@ -193,6 +188,24 @@
   </si>
   <si>
     <t>60 kg</t>
+  </si>
+  <si>
+    <t>1 USD</t>
+  </si>
+  <si>
+    <t>2 USD</t>
+  </si>
+  <si>
+    <t>3 USD</t>
+  </si>
+  <si>
+    <t>4 USD</t>
+  </si>
+  <si>
+    <t>5 USD</t>
+  </si>
+  <si>
+    <t>6 USD</t>
   </si>
 </sst>
 </file>
@@ -254,12 +267,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,12 +577,45 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="417" row="7">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+  <wetp:taskpane dockstate="right" visibility="0" width="452" row="5">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{52EAA0A0-AFDF-4F40-AA74-3BD166F316EF}">
+  <we:reference id="d170824e-af8f-4b98-8e96-baa444872b85" version="1.0.0.0" store="\\DESKTOP-OR26PFM\Users\cerdamario13\Documents\Excel Add-Ins" storeType="Filesystem"/>
+  <we:alternateReferences/>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
+<file path=xl/webextensions/webextension2.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{53392783-94BA-43D1-8995-1FED0F39B44C}">
+  <we:reference id="wa200003568" version="1.0.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="WA200003568" version="1.0.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H7"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,7 +628,7 @@
     <col min="6" max="6" width="29.42578125" customWidth="1"/>
     <col min="7" max="7" width="43.140625" customWidth="1"/>
     <col min="8" max="8" width="19.5703125" customWidth="1"/>
-    <col min="9" max="9" width="25" customWidth="1"/>
+    <col min="9" max="9" width="139.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -793,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A2EF5A-F1AF-47DC-95B5-862433988B79}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,10 +889,10 @@
         <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -859,10 +909,10 @@
         <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -879,10 +929,10 @@
         <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -899,10 +949,10 @@
         <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -919,10 +969,10 @@
         <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -939,10 +989,10 @@
         <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -951,11 +1001,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD9811B-B67A-44A4-B9F5-7DA73F13760A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{851106DF-5E1C-4561-B214-B8DF8B5B0AB6}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection sqref="A1:I7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,13 +1026,13 @@
     <col min="2" max="2" width="16.140625" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="25.28515625" customWidth="1"/>
-    <col min="5" max="6" width="36" customWidth="1"/>
-    <col min="7" max="7" width="32.5703125" customWidth="1"/>
-    <col min="8" max="8" width="38.140625" customWidth="1"/>
-    <col min="9" max="9" width="26.85546875" customWidth="1"/>
+    <col min="5" max="5" width="36" customWidth="1"/>
+    <col min="6" max="6" width="32.5703125" customWidth="1"/>
+    <col min="7" max="7" width="38.140625" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -983,23 +1045,20 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>44</v>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>111</v>
       </c>
@@ -1012,23 +1071,20 @@
       <c r="D2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E2">
-        <v>1</v>
+      <c r="E2" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="F2" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I2" t="b">
+        <v>49</v>
+      </c>
+      <c r="H2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>222</v>
       </c>
@@ -1041,23 +1097,20 @@
       <c r="D3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E3">
-        <v>2</v>
+      <c r="E3" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="F3" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="G3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I3" t="b">
+        <v>50</v>
+      </c>
+      <c r="H3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>333</v>
       </c>
@@ -1070,23 +1123,20 @@
       <c r="D4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E4">
-        <v>3</v>
+      <c r="E4" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="F4" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="G4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I4" t="b">
+        <v>51</v>
+      </c>
+      <c r="H4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>444</v>
       </c>
@@ -1099,23 +1149,20 @@
       <c r="D5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E5">
-        <v>4</v>
+      <c r="E5" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="F5" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="G5" t="s">
-        <v>48</v>
-      </c>
-      <c r="H5" t="s">
-        <v>54</v>
-      </c>
-      <c r="I5" t="b">
+        <v>52</v>
+      </c>
+      <c r="H5" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>555</v>
       </c>
@@ -1128,23 +1175,20 @@
       <c r="D6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E6">
-        <v>5</v>
+      <c r="E6" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="F6" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="G6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" t="s">
-        <v>55</v>
-      </c>
-      <c r="I6" t="b">
+        <v>53</v>
+      </c>
+      <c r="H6" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>666</v>
       </c>
@@ -1157,19 +1201,16 @@
       <c r="D7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E7">
-        <v>6</v>
+      <c r="E7" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="F7" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="G7" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I7" t="b">
+        <v>54</v>
+      </c>
+      <c r="H7" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
akeneo multiple cases for data input
</commit_message>
<xml_diff>
--- a/Akeneo Test Data.xlsx
+++ b/Akeneo Test Data.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cerdamario13\Documents\Python Files\WranglesPy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAC406C-2FFF-4A5A-A7EB-E16E9F26198D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68A6B33-1CAB-4D69-BE59-24376101257D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28020" yWindow="375" windowWidth="27735" windowHeight="11895" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Read" sheetId="1" r:id="rId1"/>
     <sheet name="Data to Write Test 1" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="11" r:id="rId3"/>
-    <sheet name="Data to Write ALL" sheetId="2" r:id="rId4"/>
+    <sheet name="Update One Value" sheetId="11" r:id="rId3"/>
+    <sheet name="Adding Another Currency" sheetId="13" r:id="rId4"/>
+    <sheet name="Data to Write ALL" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="64">
   <si>
     <t>identifier</t>
   </si>
@@ -206,6 +207,15 @@
   </si>
   <si>
     <t>6 USD</t>
+  </si>
+  <si>
+    <t>1333 USD</t>
+  </si>
+  <si>
+    <t>11.18 EUR</t>
+  </si>
+  <si>
+    <t>EUR</t>
   </si>
 </sst>
 </file>
@@ -579,7 +589,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="417" row="7">
+  <wetp:taskpane dockstate="right" visibility="0" width="413" row="7">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
   <wetp:taskpane dockstate="right" visibility="0" width="452" row="5">
@@ -1002,22 +1012,156 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD9811B-B67A-44A4-B9F5-7DA73F13760A}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="8" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1313</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1638AED3-7F47-4D94-893E-A0EF3B59A931}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="9" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>111</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{851106DF-5E1C-4561-B214-B8DF8B5B0AB6}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>